<commit_message>
Add phase1 task evidence
</commit_message>
<xml_diff>
--- a/kaizhizhang/evidence.xlsx
+++ b/kaizhizhang/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentyschan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C27926D-B025-7347-AAFC-56026F447F81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291C7E70-563C-6C47-B284-91A63FAB73D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7220" yWindow="-18220" windowWidth="19720" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9940" yWindow="-20960" windowWidth="25760" windowHeight="19920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="58">
   <si>
     <t>TxHash</t>
   </si>
@@ -167,13 +167,64 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>ibc/4935B8587058BB0FF0D7FAEEE5D9E509472367886102294316E7E1F4632D59FB</t>
+  </si>
+  <si>
+    <t>stratosgonnft2</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>BFBEA1F3859E004AEC7D60205591F68CA07BC7B1CB6B2AB8F4E1D886926D796D</t>
+  </si>
+  <si>
+    <t>3FECD57516EA4840C1942C85C0DE1F6F388AC0AEC1B66BF7708FC06AA8DED69C</t>
+  </si>
+  <si>
+    <t>C898A46BB668B957231DEEC3E3652487FC832224BAAAF069474F518CF68C339F</t>
+  </si>
+  <si>
+    <t>A26547EB65D1489EEF08974E3FEF626A7C3A57C3B4E73C7A972E8F42135EAEC0</t>
+  </si>
+  <si>
+    <t>stratosgoncollection</t>
+  </si>
+  <si>
+    <t>F7DCC664184FFBB3EF9FD504341C814BABD1095E46BBC8F0B067CB475C65B40B</t>
+  </si>
+  <si>
+    <t>stratosgonnft1</t>
+  </si>
+  <si>
+    <t>BEBBC6D6CB1CA474FEB49D5BEAD91E167B9A9CA79B2B61651546BA600F67D98D</t>
+  </si>
+  <si>
+    <t>00B313807C719CA5BBD728D5FFF56A9D6AA291FE97F4A954BED78410778FC784</t>
+  </si>
+  <si>
+    <t>stratosgonnft3</t>
+  </si>
+  <si>
+    <t>CBA8041E826F8EB915EBCBDDCC9B4CC2AA597555CAC95B5C616BD96406F2754B</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>stars18z2qwxr8w2xzn7xg5qsyyjesfhhc95zm2wkad9apamezd0eqktgqx7qyrf</t>
+  </si>
+  <si>
+    <t>stars17ypvlqnvg42zzhpk37766hlcpcllsg5e3gxf56upuu25vy088xasj7rt8t</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +240,19 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -247,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -262,6 +326,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,8 +635,8 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1093,9 +1159,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1116,6 +1184,14 @@
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1356,9 +1432,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1388,6 +1466,39 @@
         <v>16</v>
       </c>
     </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1398,9 +1509,146 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="93.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1425,10 +1673,10 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -1437,25 +1685,42 @@
         <v>12</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView zoomScale="118" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1474,10 +1739,10 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -1486,103 +1751,18 @@
         <v>12</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add phase2 task evidence
</commit_message>
<xml_diff>
--- a/kaizhizhang/evidence.xlsx
+++ b/kaizhizhang/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentyschan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaizhang/Documents/repos/gon-evidence/kaizhizhang/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291C7E70-563C-6C47-B284-91A63FAB73D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7DB257-821E-4A49-BDC6-3845C9F54BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9940" yWindow="-20960" windowWidth="25760" windowHeight="19920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-260" windowWidth="38400" windowHeight="21100" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="94">
   <si>
     <t>TxHash</t>
   </si>
@@ -58,45 +58,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -121,30 +88,6 @@
     <t>Community</t>
   </si>
   <si>
-    <t>team name</t>
-  </si>
-  <si>
-    <t>addr1</t>
-  </si>
-  <si>
-    <t>addr2</t>
-  </si>
-  <si>
-    <t>addr3</t>
-  </si>
-  <si>
-    <t>addr4</t>
-  </si>
-  <si>
-    <t>addr5</t>
-  </si>
-  <si>
-    <t>discord#1234</t>
-  </si>
-  <si>
-    <t>set none if no community</t>
-  </si>
-  <si>
     <t>stratos</t>
   </si>
   <si>
@@ -218,13 +161,178 @@
   </si>
   <si>
     <t>stars17ypvlqnvg42zzhpk37766hlcpcllsg5e3gxf56upuu25vy088xasj7rt8t</t>
+  </si>
+  <si>
+    <t>2C6B8DBAB609CA4CE2CFB91D9AAEFAB95A5C2B2D0D7BF4B2594746AF12FC7A2E</t>
+  </si>
+  <si>
+    <t>nft idstratosgonnft22</t>
+  </si>
+  <si>
+    <t>BC9B97AE5F8111E8DC5022B34A42622AF7C938DCAAE716780ACF2A9E9D20480E</t>
+  </si>
+  <si>
+    <t>stratosgonnft10</t>
+  </si>
+  <si>
+    <t>stratosgonnft21</t>
+  </si>
+  <si>
+    <t>A9C57F3CC4F5C2903E0EBE2BFBE9904F8E69F814B15949A2D7C714A4E4575285</t>
+  </si>
+  <si>
+    <t>stratosgonnft12</t>
+  </si>
+  <si>
+    <t>F36FC65D18372FE5957904E224D6D55DF1A0E1B0468367E66A0AB238B540F95B</t>
+  </si>
+  <si>
+    <t>A2255A4485E37FCF99BB2BA693E3D6F074DFAF8C44E47BB037DD702DDDE5ED34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elgafar-1 </t>
+  </si>
+  <si>
+    <t>47EA616D2C3E55080CBA289F68F7FD9B9C5033350C297A8D8343CF0F99FF2533</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>5FFEF3830375DB212D1D531D76FA9FA9ED4DD122CDBB3334BFFB0D4A98AEB3B1</t>
+  </si>
+  <si>
+    <t>6E3629F774386D0FBF2F32ADDBD358B60EBAEE69028EA7E3619F18376B53EAB7</t>
+  </si>
+  <si>
+    <t>E65CFBAC519E711936320CF47CC55602090A3B8BED0F94C153647B40C0B506C9</t>
+  </si>
+  <si>
+    <t>F6B04649C69CDB61C2D08E74B8EAC45037C7D69EED934AEC3AF5D5B9D92BED12</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>2B7CC4392C8AEEF47D86DB1CE95D700A5528AE3B9549315F449834CE6564F8D3</t>
+  </si>
+  <si>
+    <t>358653DB905A48D83619DFDDBE9150161B79BFB0C57CB4C852B3E0C0D1630670</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gon-irishub-1 </t>
+  </si>
+  <si>
+    <t>0D8ED0D1047812B01A51DE6472D5CFD0BE6511547509530A3DFAEAF45E3424FB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uni-6 </t>
+  </si>
+  <si>
+    <t>E0F7F2ED859F75EE89AC898A4B8220F6AB0C2A4B64BCA5EB53DF5A86A58FBDA4</t>
+  </si>
+  <si>
+    <t>6D1CA2815FE6D183E7C4C6DC51C8255474142292B3107EEFF9BEFB7CE7B537C4</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>43F203DDCB8A2C54993FA9DAF7044174EFD9F869AEAA48C338AEFBC7A1D883B6</t>
+  </si>
+  <si>
+    <t>9BBF319F5DE4B0D2425C7C0FA26D2F28F990E953773224A274B2D0CF8513CB82</t>
+  </si>
+  <si>
+    <t>F2989480949F8E134D66B8C7421F8D7C33BB14B9B2BC3EEB4D3FD022A31BE761</t>
+  </si>
+  <si>
+    <t>A5DC0D2E4A192D986ED414BF0F4B74C4E5E1EF98878AA759763898745F629F37</t>
+  </si>
+  <si>
+    <t>26E30F5C0BCECF5B78CD07AEF830DC3E465C2C4E9AD893824AC97C057F6A4A66</t>
+  </si>
+  <si>
+    <t>chain idgon-irishub-1</t>
+  </si>
+  <si>
+    <t>D705C816E2DF2B6804524255D8F7FCA8F77E9CF2E68C21761956489C25E44BC4</t>
+  </si>
+  <si>
+    <t>92DEF447EA380D072E0ACACCCA41C03C7A66421651B7C7D4DB4B3D88DDFACE95</t>
+  </si>
+  <si>
+    <t>D3F80432EC98778771A3DF20023A5AA4CEB67117DE7D5C5E2A253AEBACF0D826</t>
+  </si>
+  <si>
+    <t>3D9FCFD95F0FCDDF2E3EE0C0D166DDF9E9756D69EC0E8754172E99DF81666D77</t>
+  </si>
+  <si>
+    <t>53220990B20225DF9CBDF2E82024BA497BA43033AFF6F7335FD60495FBCE8695</t>
+  </si>
+  <si>
+    <t>7E575FC4B4C5DA0449D719AF65C68B1D36270DC01BC25BFFAB232111A5363157</t>
+  </si>
+  <si>
+    <t>2C4BAD4419D19B8AEF1B615124CC4C7A030BA8998940C9693A4EF621F00A599B</t>
+  </si>
+  <si>
+    <t>B37604227272B2FBD44123C05DFBBE00C8A7A671C6948BD4E28E6471E1558837</t>
+  </si>
+  <si>
+    <t>587F4CAFC44D7FF1157D50557C8C0C7D7A700FD2226A2554BF51E3B6CB296EF9</t>
+  </si>
+  <si>
+    <t>281502B002CE4BA1A28A34EE768CF503F8446CCD9314E23762D51A49EDB1183F</t>
+  </si>
+  <si>
+    <t>69C3634A858DBB9AF9F9A62930AC11569E1C45887A10BC39373F504877FCE118</t>
+  </si>
+  <si>
+    <t>96E99F3583E22B7FEE58E463302D51822C481F4E0EA374FFBCC5AB4BE8E424D3</t>
+  </si>
+  <si>
+    <t>F3F20C368273AB3B02A90A89FB328D3D83E5F624F1D86A123B0BEB37731707A7</t>
+  </si>
+  <si>
+    <t>2D47D1BB262C5611BFFBC8BE4F4CBFB861E6F469A2F5637C645AFC16A04AC7BF</t>
+  </si>
+  <si>
+    <t>C9B6B2EA8E88EBF43272E9DFD0F8D6EA08D5D5D386BD843E41E3FAB6E0B58A94</t>
+  </si>
+  <si>
+    <t>DFC003041EA370B0ABEC73C9FA79FA620BC71AF02717C709CB150AC482CE6EBA</t>
+  </si>
+  <si>
+    <t>BCB294FD884ABD76EDC4FAF63D438D1FA964735AE739F45B17E8E17B786C79E8</t>
+  </si>
+  <si>
+    <t>9FD55A55B72DDC869D8B1F06712451D3CEDC1585F8B4E6465807834D066ED532</t>
+  </si>
+  <si>
+    <t>elgafar-1 </t>
+  </si>
+  <si>
+    <t>9A174447FCF3690210DC0A0AD001EE95B5EEF51E1BBB1995FCE8E594284248DC</t>
+  </si>
+  <si>
+    <t>BC5AEE9AF162081BBA8EF3B6CFAB86E3CD48A25407359F6733E68AA89F6841DF</t>
+  </si>
+  <si>
+    <t>DF63F2EE7F7C3D5B83B5C1E0ABFE334E6AAB81067DB4A243A173C3B66AA83317</t>
+  </si>
+  <si>
+    <t>stratosgonnft7</t>
+  </si>
+  <si>
+    <t>995FEBFE2B0BE3B7CF33CDDA38B0845C514F5D55E002F0F53CBF402FC7F31581</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,8 +366,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,11 +383,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -311,15 +420,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -328,6 +434,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,7 +745,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -645,7 +754,7 @@
     <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
@@ -653,81 +762,65 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -741,7 +834,47 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="77.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -751,33 +884,73 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+        <v>93</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -787,33 +960,35 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <c r="A2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -823,33 +998,59 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <c r="A2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -859,33 +1060,59 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <c r="A2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -902,36 +1129,52 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
+      <c r="A3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <c r="A4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -948,36 +1191,52 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
+      <c r="A3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <c r="A4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -994,36 +1253,52 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
+      <c r="A2" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
+      <c r="A3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <c r="A4" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1040,36 +1315,89 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1086,36 +1414,68 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
+      <c r="A3" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <c r="A4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1132,158 +1492,51 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
+      <c r="A3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
+      <c r="A4" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1432,7 +1685,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -1449,54 +1702,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
+      <c r="A2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>50</v>
+      <c r="A3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>53</v>
+      <c r="A4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1512,7 +1754,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1528,45 +1770,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>55</v>
+      <c r="A2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B6" s="6"/>
+      <c r="B6" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1578,10 +1806,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1597,41 +1825,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1644,10 +1858,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1662,41 +1876,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>43</v>
+      <c r="A2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1709,10 +1909,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1728,41 +1928,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1777,7 +1963,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1787,18 +1975,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+      <c r="A2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1813,7 +2001,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1823,18 +2013,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+      <c r="A2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>